<commit_message>
sources for note on Matuschak
</commit_message>
<xml_diff>
--- a/coronavirus-extrapolations.xlsx
+++ b/coronavirus-extrapolations.xlsx
@@ -64,7 +64,7 @@
     <numFmt numFmtId="60" formatCode="#,##0.0"/>
     <numFmt numFmtId="61" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -90,11 +90,6 @@
     <font>
       <sz val="10"/>
       <color indexed="13"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="14"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -243,7 +238,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -262,10 +257,10 @@
     <xf numFmtId="59" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -274,10 +269,7 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -286,7 +278,7 @@
     <xf numFmtId="3" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -295,7 +287,7 @@
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="60" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -337,7 +329,6 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="fff27100"/>
       <rgbColor rgb="ffd69500"/>
     </indexedColors>
   </colors>
@@ -1462,7 +1453,7 @@
         <v>43965</v>
       </c>
       <c r="B3" s="6">
-        <v>85800</v>
+        <v>87000</v>
       </c>
       <c r="C3" s="7">
         <f>I3*J3</f>
@@ -1476,491 +1467,492 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>1440000</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>43958</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>76928</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <f>I4*J4</f>
         <v>9436147.9</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <f>C7*1.5</f>
         <v>9578400</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="15">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14">
         <v>1292623</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <v>7.3</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>43951</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>63856</v>
       </c>
       <c r="C5" s="14">
-        <f>I5*J5</f>
-        <v>8541179.4</v>
-      </c>
-      <c r="D5" s="15">
+        <f>100*B3</f>
+        <v>8700000</v>
+      </c>
+      <c r="D5" s="14">
         <f>C8*1.5</f>
         <v>7535400</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="15">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14">
         <v>1095023</v>
       </c>
       <c r="J5" s="17">
-        <v>7.8</v>
+        <f>C5/I5</f>
+        <v>7.9450385973628</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>43944</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>50236</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <f>100*B4</f>
         <v>7692800</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>C9*1.5</f>
         <v>5192550</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f>3*C9</f>
         <v>10385100</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="15">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14">
         <v>886442</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <f>C6/I6</f>
         <v>8.67828916048653</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>43937</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>34617</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <f>100*B5</f>
         <v>6385600</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <f>C10*1.5</f>
         <v>2506800</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f>3*C10</f>
         <v>5013600</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <f>6*C10</f>
         <v>10027200</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="15">
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
         <v>639664</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="17">
         <f>C7/I7</f>
         <v>9.98274093899297</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <f>$A7-7</f>
         <v>43930</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>16712</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <f>100*B6</f>
         <v>5023600</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <f>C11*1.5</f>
         <v>913200</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f>3*C11</f>
         <v>1826400</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <f>6*C11</f>
         <v>3652800</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <f>F8*2</f>
         <v>7305600</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15">
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>432132</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <f>C8/I8</f>
         <v>11.6251515740561</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <f>$A8-7</f>
         <v>43923</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>6088</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <f>100*B7</f>
         <v>3461700</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <f>C12*1.5</f>
         <v>194400</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <f>3*C12</f>
         <v>388800</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <f>6*C12</f>
         <v>777600</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <f>F9*2</f>
         <v>1555200</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="15">
+      <c r="H9" s="15"/>
+      <c r="I9" s="14">
         <v>216721</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <f>C9/I9</f>
         <v>15.9730713682569</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <f>$A9-7</f>
         <v>43916</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>1296</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <f>100*B8</f>
         <v>1671200</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <f>C13*1.5</f>
         <v>30900</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <f>3*C13</f>
         <v>61800</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f>6*C13</f>
         <v>123600</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <f>F10*2</f>
         <v>247200</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="15">
+      <c r="H10" s="15"/>
+      <c r="I10" s="14">
         <v>69194</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="17">
         <f>C10/I10</f>
         <v>24.1523831546088</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <f>$A10-7</f>
         <v>43909</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>206</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <f>100*B9</f>
         <v>608800</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <f>C14*1.5</f>
         <v>6150</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <f>3*C14</f>
         <v>12300</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f>6*C14</f>
         <v>24600</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <f>F11*2</f>
         <v>49200</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="15">
+      <c r="H11" s="15"/>
+      <c r="I11" s="14">
         <v>9415</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="17">
         <f>C11/I11</f>
         <v>64.6627721720659</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <f>$A11-7</f>
         <v>43902</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>41</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <f>100*B10</f>
         <v>129600</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <f>C15*1.5</f>
         <v>1800</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <f>3*C15</f>
         <v>3600</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <f>6*C15</f>
         <v>7200</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <f>F12*2</f>
         <v>14400</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="15">
+      <c r="H12" s="15"/>
+      <c r="I12" s="14">
         <v>1312</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="17">
         <f>C12/I12</f>
         <v>98.78048780487801</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <f>$A12-7</f>
         <v>43895</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>12</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <f>100*B11</f>
         <v>20600</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <f>C16*1.5</f>
         <v>150</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <f>3*C16</f>
         <v>300</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f>6*C16</f>
         <v>600</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <f>F13*2</f>
         <v>1200</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="15">
+      <c r="H13" s="15"/>
+      <c r="I13" s="14">
         <v>159</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="17">
         <f>C13/I13</f>
         <v>129.559748427673</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <f>$A13-7</f>
         <v>43888</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>1</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <f>100*B12</f>
         <v>4100</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14">
         <v>59</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <f>C14/I14</f>
         <v>69.4915254237288</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <f>$A14-7</f>
         <v>43881</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="15">
+      <c r="B15" s="12"/>
+      <c r="C15" s="14">
         <f>100*B13</f>
         <v>1200</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14">
         <v>15</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <f>C15/I15</f>
         <v>80</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <f>$A15-7</f>
         <v>43874</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="15">
+      <c r="B16" s="12"/>
+      <c r="C16" s="14">
         <f>100*B14</f>
         <v>100</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14">
         <v>14</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="17">
         <f>C16/I16</f>
         <v>7.14285714285714</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="12">
+      <c r="A17" s="11">
         <f>$A16-7</f>
         <v>43867</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19">
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18">
         <v>12</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="17">
         <f>C17/I17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="12">
+      <c r="A18" s="11">
         <f>$A17-7</f>
         <v>43860</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19">
+      <c r="B18" s="12"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18">
         <v>5</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="17">
         <f>C18/I18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18">
         <v>1</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="17">
         <f>C19/I19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" t="s" s="22">
+      <c r="A20" s="19"/>
+      <c r="B20" t="s" s="21">
         <v>10</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="23"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>